<commit_message>
(frontend): finished book creation page, with loading animation and data fetching. Next milestone: refactor backend to seperate image generations from pdf creation
</commit_message>
<xml_diff>
--- a/cb_frontend/public/locales/translations.xlsx
+++ b/cb_frontend/public/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\MyLocalFiles\WebProgramming\colouringbook\cb_frontend\public\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C32717-FE08-43D4-AC6F-94F14A297D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1501A8DA-CCDA-47A8-BD3A-450CBCD17018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9BF5BC8-2BED-48F5-A248-5FD17E4967B8}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>key</t>
   </si>
   <si>
-    <t>en-gb</t>
-  </si>
-  <si>
     <t>fr</t>
   </si>
   <si>
@@ -144,6 +141,81 @@
   </si>
   <si>
     <t>Una partita di calcio dove i simpatici conigli vincono contro i cani cattivi</t>
+  </si>
+  <si>
+    <t>creation.placeholder</t>
+  </si>
+  <si>
+    <t>Mario playing with…</t>
+  </si>
+  <si>
+    <t>creation.option1</t>
+  </si>
+  <si>
+    <t>Mario jouant avec...</t>
+  </si>
+  <si>
+    <t>Mario spielt mit...</t>
+  </si>
+  <si>
+    <t>Mario gioca con...</t>
+  </si>
+  <si>
+    <t>Mario jugando con...</t>
+  </si>
+  <si>
+    <t>Meilleure qualité d'image (augmentation du prix)</t>
+  </si>
+  <si>
+    <t>Better quality (increased price)</t>
+  </si>
+  <si>
+    <t>Bessere Bildqualität (Preiserhöhung)</t>
+  </si>
+  <si>
+    <t>Migliore qualità dell'immagine (aumento del prezzo)</t>
+  </si>
+  <si>
+    <t>Mejor calidad de imagen (aumento de precio)</t>
+  </si>
+  <si>
+    <t>creation.option2</t>
+  </si>
+  <si>
+    <t>Coloriage plus difficile</t>
+  </si>
+  <si>
+    <t>More difficult colouring</t>
+  </si>
+  <si>
+    <t>Schwierigeres Ausmalen</t>
+  </si>
+  <si>
+    <t>Colorazione più difficile</t>
+  </si>
+  <si>
+    <t>Colorear más difícil</t>
+  </si>
+  <si>
+    <t>creation.option3</t>
+  </si>
+  <si>
+    <t>Only one page</t>
+  </si>
+  <si>
+    <t>Une seule page</t>
+  </si>
+  <si>
+    <t>Nur eine Seite</t>
+  </si>
+  <si>
+    <t>Solo una pagina</t>
+  </si>
+  <si>
+    <t>Solo una página</t>
+  </si>
+  <si>
+    <t>en_gb</t>
   </si>
 </sst>
 </file>
@@ -521,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20738A67-AA73-454B-8B08-FEE60033B2E5}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -541,119 +613,199 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
(frontend): fully implemented a help drop down page in creation page
</commit_message>
<xml_diff>
--- a/cb_frontend/public/locales/translations.xlsx
+++ b/cb_frontend/public/locales/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\MyLocalFiles\WebProgramming\colouringbook\cb_frontend\public\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1501A8DA-CCDA-47A8-BD3A-450CBCD17018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C37721-15C6-4C74-9769-25BD5B844034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9BF5BC8-2BED-48F5-A248-5FD17E4967B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>key</t>
   </si>
@@ -143,18 +143,9 @@
     <t>Una partita di calcio dove i simpatici conigli vincono contro i cani cattivi</t>
   </si>
   <si>
-    <t>creation.placeholder</t>
-  </si>
-  <si>
-    <t>Mario playing with…</t>
-  </si>
-  <si>
     <t>creation.option1</t>
   </si>
   <si>
-    <t>Mario jouant avec...</t>
-  </si>
-  <si>
     <t>Mario spielt mit...</t>
   </si>
   <si>
@@ -216,13 +207,148 @@
   </si>
   <si>
     <t>en_gb</t>
+  </si>
+  <si>
+    <t>creation.create</t>
+  </si>
+  <si>
+    <t>Create my book</t>
+  </si>
+  <si>
+    <t>Créer mon livre</t>
+  </si>
+  <si>
+    <t>Erstelle mein Buch</t>
+  </si>
+  <si>
+    <t>Crea il mio libro</t>
+  </si>
+  <si>
+    <t>Crea mi libro</t>
+  </si>
+  <si>
+    <t>creation.warning1</t>
+  </si>
+  <si>
+    <t>Please fill in the book description!</t>
+  </si>
+  <si>
+    <t>Veuillez remplir la description de votre livre!</t>
+  </si>
+  <si>
+    <t>creation.placeholder1</t>
+  </si>
+  <si>
+    <t>creation.placeholder2</t>
+  </si>
+  <si>
+    <t>creation.placeholder3</t>
+  </si>
+  <si>
+    <t>creation.tips1</t>
+  </si>
+  <si>
+    <t>creation.tips2</t>
+  </si>
+  <si>
+    <t>creation.tips3</t>
+  </si>
+  <si>
+    <t>creation.tips4</t>
+  </si>
+  <si>
+    <t>creation.tips5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A rabbit in a football outfit scoring a goal. The football is in the bottom corner of the goal net. The big text "GOAL" is written on top of the page. 
+A happy gnome sat on a tree stump and eating pizza. </t>
+  </si>
+  <si>
+    <t>Mario playing chess against a frog in a park, they are both focused and having fun.
+A dragon blowing the candled on his birthday cake.</t>
+  </si>
+  <si>
+    <t>A group of three frogs jumping over the moon.
+A big, open, glowing treasure-chest full of pizza and ice cream.</t>
+  </si>
+  <si>
+    <t>Mario jouant aux échecs contre une grenouille dans un parc, ils sont tous les deux concentrés et s'amusent. 
+Un dragon soufflant sur les bougies de son gâteau d'anniversaire.</t>
+  </si>
+  <si>
+    <t>Un lapin en tenue de football marquant un but. Le ballon est dans le coin inférieur du filet. Le grand texte « BUT » est écrit en haut de la page. 
+Un gnome heureux assis sur une souche d'arbre en train de manger une pizza.</t>
+  </si>
+  <si>
+    <t>Un groupe de trois grenouilles sautant par-dessus la lune.
+Un grand coffre au trésor ouvert, brillant et rempli de pizzas et de glaces.</t>
+  </si>
+  <si>
+    <t>Generate multiple pages by writing each scene in a separate sentence.
+ [do] A dragon blowing the candled on his birthday cake. 
+A heard of 5 happy sheep in a field, watching TV on a big screen[/do]</t>
+  </si>
+  <si>
+    <t>Use specific descriptions
+[avoid]…playing together[/avoid] [do]…playing catch and running around in a grass field[/do] [avoid]some dogs[/avoid] [do]a group of three dogs[/do]</t>
+  </si>
+  <si>
+    <t>For more complicated scenes or better quality, toggle "Better quality"</t>
+  </si>
+  <si>
+    <t>Avoid putting too many characters together [avoid]…with a dragon, an elephant, a crocodile, a gnome, a witch[/avoid] [do]...with a gnome sitting besides a dragon.[/do]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Famous characters/people can give inconsistent results
+[avoid] Mario, Superman, Elon Musk[/avoid] 
+[do]dog, dragon, gnome, fairy, tall man with a moustache, smiling man with big wavy yellow hair[/do] 
+</t>
+  </si>
+  <si>
+    <t>Générez plusieurs pages en écrivant chaque scène dans une phrase distincte
+[do]Un dragon soufflant sur les bougies de son gâteau d'anniversaire. Un troupeau de 5 moutons heureux dans un champ, regardant la télévision sur un grand écran[/do]</t>
+  </si>
+  <si>
+    <t>Les personnages/personnes célèbres peuvent donner des résultats incohérents
+[avoid]Mario, Superman, Elon Musk[/avoid]
+[do]Un chien, un dragon, un gnome, une fée, un homme grand avec une moustache, un homme souriant avec de grands cheveux jaunes ondulés[/do]</t>
+  </si>
+  <si>
+    <t>Pour des scènes plus complexes ou une meilleure qualité, activez "Meilleure qualité"</t>
+  </si>
+  <si>
+    <t>Utilisez des descriptions spécifiques. 
+[avoid]…jouant ensemble[/avoid][do]…jouant au loup et courant dans un grand champ d'herbe[/do] 
+[avoid]des chiens[/avoid]  [do] un groupe de trois chiens[/do]</t>
+  </si>
+  <si>
+    <t>Évitez de regrouper trop de personnages
+[avoid]…avec un dragon, un grand éléphant, un crocodile et un lutin heureux[/avoid] [do]avec un lutin assis à côté d’un dragon.[/do]</t>
+  </si>
+  <si>
+    <t>creation.tips_button</t>
+  </si>
+  <si>
+    <t>Help! How do I make my book?</t>
+  </si>
+  <si>
+    <t>Aide: Comment créer son livre?</t>
+  </si>
+  <si>
+    <t>creation.tips_close_button</t>
+  </si>
+  <si>
+    <t>Click again to hide</t>
+  </si>
+  <si>
+    <t>Cliquez à nouveau pour masquer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +360,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Bu-Wicked"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -256,9 +388,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,19 +730,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20738A67-AA73-454B-8B08-FEE60033B2E5}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" customWidth="1"/>
-    <col min="2" max="2" width="72" customWidth="1"/>
-    <col min="3" max="3" width="69.42578125" customWidth="1"/>
-    <col min="4" max="4" width="81.5703125" customWidth="1"/>
+    <col min="1" max="4" width="50.7109375" customWidth="1"/>
     <col min="5" max="5" width="69.140625" customWidth="1"/>
+    <col min="6" max="6" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -613,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -628,187 +763,344 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="30">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="60">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>58</v>
+    </row>
+    <row r="16" spans="1:6" ht="75">
+      <c r="A16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="60">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="105">
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" ht="105">
+      <c r="A21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="75">
+      <c r="A22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="60">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30">
+      <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(UI): added scribble text and tiling scribble background
</commit_message>
<xml_diff>
--- a/cb_frontend/public/locales/translations.xlsx
+++ b/cb_frontend/public/locales/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\MyLocalFiles\WebProgramming\colouringbook\cb_frontend\public\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C37721-15C6-4C74-9769-25BD5B844034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F428C715-19EC-48C5-BABF-C08AF8FEA606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9BF5BC8-2BED-48F5-A248-5FD17E4967B8}"/>
   </bookViews>
@@ -155,21 +155,6 @@
     <t>Mario jugando con...</t>
   </si>
   <si>
-    <t>Meilleure qualité d'image (augmentation du prix)</t>
-  </si>
-  <si>
-    <t>Better quality (increased price)</t>
-  </si>
-  <si>
-    <t>Bessere Bildqualität (Preiserhöhung)</t>
-  </si>
-  <si>
-    <t>Migliore qualità dell'immagine (aumento del prezzo)</t>
-  </si>
-  <si>
-    <t>Mejor calidad de imagen (aumento de precio)</t>
-  </si>
-  <si>
     <t>creation.option2</t>
   </si>
   <si>
@@ -342,6 +327,21 @@
   </si>
   <si>
     <t>Cliquez à nouveau pour masquer</t>
+  </si>
+  <si>
+    <t>Meilleure qualité</t>
+  </si>
+  <si>
+    <t>Better quality</t>
+  </si>
+  <si>
+    <t>Bessere Bildqualität</t>
+  </si>
+  <si>
+    <t>Migliore qualità dell'immagine</t>
+  </si>
+  <si>
+    <t>Mejor calidad de imagen</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20738A67-AA73-454B-8B08-FEE60033B2E5}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +748,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -884,110 +884,110 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
         <v>57</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60">
       <c r="A15" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -1001,102 +1001,102 @@
     </row>
     <row r="16" spans="1:6" ht="75">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="105">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" ht="105">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: update all tranlsations
</commit_message>
<xml_diff>
--- a/cb_frontend/public/locales/translations.xlsx
+++ b/cb_frontend/public/locales/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\MyLocalFiles\WebProgramming\colouringbook\cb_frontend\public\locales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F428C715-19EC-48C5-BABF-C08AF8FEA606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63552638-C1E9-429E-84F4-46337FB235A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E9BF5BC8-2BED-48F5-A248-5FD17E4967B8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>key</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Solo una página</t>
-  </si>
-  <si>
-    <t>en_gb</t>
   </si>
   <si>
     <t>creation.create</t>
@@ -342,13 +339,214 @@
   </si>
   <si>
     <t>Mejor calidad de imagen</t>
+  </si>
+  <si>
+    <t>modifybook.credits.out_of_credits</t>
+  </si>
+  <si>
+    <t>Out of credits!</t>
+  </si>
+  <si>
+    <t>Plus de crédits !</t>
+  </si>
+  <si>
+    <t>Keine Guthaben mehr!</t>
+  </si>
+  <si>
+    <t>Crediti esauriti!</t>
+  </si>
+  <si>
+    <t>¡Sin créditos!</t>
+  </si>
+  <si>
+    <t>modifybook.processing</t>
+  </si>
+  <si>
+    <t>Processing...</t>
+  </si>
+  <si>
+    <t>Traitement en cours...</t>
+  </si>
+  <si>
+    <t>Verarbeitung...</t>
+  </si>
+  <si>
+    <t>Elaborazione in corso...</t>
+  </si>
+  <si>
+    <t>Procesando...</t>
+  </si>
+  <si>
+    <t>modifybook.download_pdf</t>
+  </si>
+  <si>
+    <t>Download PDF</t>
+  </si>
+  <si>
+    <t>Télécharger le PDF</t>
+  </si>
+  <si>
+    <t>PDF herunterladen</t>
+  </si>
+  <si>
+    <t>Scarica PDF</t>
+  </si>
+  <si>
+    <t>Descargar PDF</t>
+  </si>
+  <si>
+    <t>modifybook.finish_book</t>
+  </si>
+  <si>
+    <t>Finish Book</t>
+  </si>
+  <si>
+    <t>Terminer le livre</t>
+  </si>
+  <si>
+    <t>Buch abschließen</t>
+  </si>
+  <si>
+    <t>Completa il libro</t>
+  </si>
+  <si>
+    <t>Terminar libro</t>
+  </si>
+  <si>
+    <t>modifybook.creative_model</t>
+  </si>
+  <si>
+    <t>Creative Model</t>
+  </si>
+  <si>
+    <t>Modèle créatif</t>
+  </si>
+  <si>
+    <t>Kreatives Modell</t>
+  </si>
+  <si>
+    <t>Modello creativo</t>
+  </si>
+  <si>
+    <t>Modelo creativo</t>
+  </si>
+  <si>
+    <t>modifybook.creative_model_description</t>
+  </si>
+  <si>
+    <t>More creative images, but may include extra shading and details</t>
+  </si>
+  <si>
+    <t>Images plus créatives, mais peuvent inclure des ombrages et des détails supplémentaires</t>
+  </si>
+  <si>
+    <t>Kreativere Bilder, können jedoch zusätzliche Schattierungen und Details enthalten</t>
+  </si>
+  <si>
+    <t>Immagini più creative, ma possono includere ulteriori sfumature e dettagli</t>
+  </si>
+  <si>
+    <t>Imágenes más creativas, pero pueden incluir sombreado extra y detalles</t>
+  </si>
+  <si>
+    <t>modifybook.advanced_options</t>
+  </si>
+  <si>
+    <t>Advanced Options</t>
+  </si>
+  <si>
+    <t>Options avancées</t>
+  </si>
+  <si>
+    <t>Erweiterte Optionen</t>
+  </si>
+  <si>
+    <t>Opzioni avanzate</t>
+  </si>
+  <si>
+    <t>Opciones avanzadas</t>
+  </si>
+  <si>
+    <t>modifybook.test_mode</t>
+  </si>
+  <si>
+    <t>Test Mode</t>
+  </si>
+  <si>
+    <t>Mode test</t>
+  </si>
+  <si>
+    <t>Testmodus</t>
+  </si>
+  <si>
+    <t>Modalità test</t>
+  </si>
+  <si>
+    <t>Modo de prueba</t>
+  </si>
+  <si>
+    <t>modifybook.test_mode_description</t>
+  </si>
+  <si>
+    <t>Show descriptions instead of generating images</t>
+  </si>
+  <si>
+    <t>Afficher les descriptions au lieu de générer des images</t>
+  </si>
+  <si>
+    <t>Zeige Beschreibungen anstelle von Bildern</t>
+  </si>
+  <si>
+    <t>Mostra descrizioni invece di generare immagini</t>
+  </si>
+  <si>
+    <t>Mostrar descripciones en lugar de generar imágenes</t>
+  </si>
+  <si>
+    <t>modifybook.advanced_story_context</t>
+  </si>
+  <si>
+    <t>Advanced Story Context</t>
+  </si>
+  <si>
+    <t>Contexte d'histoire avancé</t>
+  </si>
+  <si>
+    <t>Erweiterter Story-Kontext</t>
+  </si>
+  <si>
+    <t>Contesto storia avanzato</t>
+  </si>
+  <si>
+    <t>Contexto de historia avanzado</t>
+  </si>
+  <si>
+    <t>modifybook.advanced_story_context_description</t>
+  </si>
+  <si>
+    <t>Use more detailed story context for better continuity</t>
+  </si>
+  <si>
+    <t>Utiliser un contexte d'histoire plus détaillé pour une meilleure continuité</t>
+  </si>
+  <si>
+    <t>Verwenden Sie einen detaillierteren Story-Kontext für bessere Kontinuität</t>
+  </si>
+  <si>
+    <t>Usa un contesto di storia più dettagliato per una migliore continuità</t>
+  </si>
+  <si>
+    <t>Usar un contexto de historia más detallado para una mejor continuidad</t>
+  </si>
+  <si>
+    <t>en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +561,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,13 +594,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20738A67-AA73-454B-8B08-FEE60033B2E5}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>161</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -884,19 +1096,19 @@
         <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -941,53 +1153,53 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>55</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>56</v>
-      </c>
-      <c r="F13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="60">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>36</v>
@@ -1001,102 +1213,330 @@
     </row>
     <row r="16" spans="1:6" ht="75">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60">
+      <c r="A17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="60">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="105">
+      <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="105">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="105">
+      <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75">
+      <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" ht="105">
-      <c r="A21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="60">
+      <c r="A23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="30">
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="75">
-      <c r="A22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="60">
-      <c r="A23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
-      <c r="A24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>82</v>
+    <row r="27" spans="1:6">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
+      <c r="A33" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="A38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>